<commit_message>
hard + removed fallback weights
</commit_message>
<xml_diff>
--- a/eval/responses/claude-opus-4-5-20251101/20260113_215424/h-001_output_1.xlsx
+++ b/eval/responses/claude-opus-4-5-20251101/20260113_215424/h-001_output_1.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\Mac\Home\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\Mac\Home\Code\ib-bench\eval\responses\claude-opus-4-5-20251101\20260113_215424\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F0688AD-6375-43FE-BA49-C168C95A93C5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E2D3FB1-C3C9-4E06-B9BB-733126572AF5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="22920" windowHeight="14475" tabRatio="500" firstSheet="2" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="330" windowWidth="29040" windowHeight="15990" tabRatio="500" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Output" sheetId="1" r:id="rId1"/>
@@ -2491,7 +2491,7 @@
   <dimension ref="A1:T38"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+      <selection activeCell="K18" sqref="K18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="15.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2847,7 +2847,7 @@
       </c>
       <c r="S18" s="26">
         <f ca="1">+R18/$R$22</f>
-        <v>1.6424375133342547E-2</v>
+        <v>1.6424375133342464E-2</v>
       </c>
       <c r="T18" s="27">
         <f ca="1">+$R$22*S18</f>
@@ -2896,19 +2896,19 @@
       </c>
       <c r="Q19" s="30">
         <f ca="1">+'P&amp;L'!M72</f>
-        <v>0.17747281390745021</v>
+        <v>0.17747281390745012</v>
       </c>
       <c r="R19" s="15">
         <f ca="1">+(Q19-P19)*Q18*P20/$M$31</f>
-        <v>1.7478450899726825</v>
+        <v>1.7478450899726783</v>
       </c>
       <c r="S19" s="26">
         <f ca="1">+R19/$R$22</f>
-        <v>4.4154183891837701E-2</v>
+        <v>4.4154183891837361E-2</v>
       </c>
       <c r="T19" s="27">
         <f ca="1">+$R$22*S19</f>
-        <v>1.7478450899726825</v>
+        <v>1.7478450899726783</v>
       </c>
     </row>
     <row r="20" spans="2:20" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -2935,7 +2935,7 @@
       </c>
       <c r="M20" s="32">
         <f ca="1">+'P&amp;L'!M71</f>
-        <v>99.029830160357207</v>
+        <v>99.029830160357164</v>
       </c>
       <c r="O20" s="15" t="s">
         <v>29</v>
@@ -2946,19 +2946,19 @@
       </c>
       <c r="Q20" s="33">
         <f ca="1">+M26</f>
-        <v>82.702353288277919</v>
+        <v>82.702353288277735</v>
       </c>
       <c r="R20" s="15">
         <f ca="1">+(Q20-P20)*Q19*Q18/$M$31</f>
-        <v>38.421095495883961</v>
+        <v>38.42109549588384</v>
       </c>
       <c r="S20" s="26">
         <f ca="1">+R20/$R$22</f>
-        <v>0.97059637926930453</v>
+        <v>0.97059637926929643</v>
       </c>
       <c r="T20" s="27">
         <f ca="1">+$R$22*S20</f>
-        <v>38.421095495883961</v>
+        <v>38.42109549588384</v>
       </c>
     </row>
     <row r="21" spans="2:20" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -2978,15 +2978,15 @@
       <c r="Q21" s="15"/>
       <c r="R21" s="15">
         <f ca="1">+R22-SUM(R18:R20)</f>
-        <v>-1.2340611472220999</v>
+        <v>-1.234061147221766</v>
       </c>
       <c r="S21" s="26">
         <f ca="1">+R21/$R$22</f>
-        <v>-3.1174938294484904E-2</v>
+        <v>-3.1174938294476307E-2</v>
       </c>
       <c r="T21" s="27">
         <f ca="1">+$R$22*S21</f>
-        <v>-1.2340611472220999</v>
+        <v>-1.234061147221766</v>
       </c>
     </row>
     <row r="22" spans="2:20" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -3025,7 +3025,7 @@
       <c r="Q22" s="31"/>
       <c r="R22" s="35">
         <f ca="1">+M33-D18</f>
-        <v>39.585038968318443</v>
+        <v>39.585038968318386</v>
       </c>
       <c r="S22" s="15"/>
       <c r="T22" s="15"/>
@@ -3118,7 +3118,7 @@
       </c>
       <c r="M26" s="39">
         <f ca="1">+M24/M20</f>
-        <v>82.702353288277706</v>
+        <v>82.702353288277735</v>
       </c>
     </row>
     <row r="27" spans="2:20" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -3159,7 +3159,7 @@
       </c>
       <c r="M28" s="25">
         <f ca="1">+'BS &amp; CFS'!M50</f>
-        <v>851.41875458408856</v>
+        <v>851.41875458408629</v>
       </c>
     </row>
     <row r="29" spans="2:20" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -3178,7 +3178,7 @@
       </c>
       <c r="M29" s="32">
         <f ca="1">+M24-M28</f>
-        <v>7338.5812454159113</v>
+        <v>7338.5812454159141</v>
       </c>
     </row>
     <row r="30" spans="2:20" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -3232,7 +3232,7 @@
       </c>
       <c r="M33" s="42">
         <f ca="1">+M29/M31</f>
-        <v>42.395038968318381</v>
+        <v>42.395038968318396</v>
       </c>
     </row>
     <row r="34" spans="2:17" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -3251,7 +3251,7 @@
       </c>
       <c r="M34" s="44">
         <f ca="1">+M33/$D$18-1</f>
-        <v>14.087202479828605</v>
+        <v>14.08720247982861</v>
       </c>
     </row>
     <row r="35" spans="2:17" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -3270,7 +3270,7 @@
       </c>
       <c r="M35" s="43">
         <f ca="1">+M33/$D$18</f>
-        <v>15.087202479828605</v>
+        <v>15.08720247982861</v>
       </c>
       <c r="Q35" s="45"/>
     </row>
@@ -4104,31 +4104,31 @@
       </c>
       <c r="M17">
         <f t="shared" ref="M17:S17" ca="1" si="5">+(M14-M19)*-1</f>
-        <v>-108.62957661127942</v>
+        <v>-108.62957661127948</v>
       </c>
       <c r="N17">
         <f t="shared" ca="1" si="5"/>
-        <v>-114.39957493058509</v>
+        <v>-114.39957493058338</v>
       </c>
       <c r="O17">
         <f t="shared" ca="1" si="5"/>
-        <v>-120.46879706454979</v>
+        <v>-120.46879706457116</v>
       </c>
       <c r="P17">
         <f t="shared" ca="1" si="5"/>
-        <v>-148.25687584617623</v>
+        <v>-148.25687584598768</v>
       </c>
       <c r="Q17">
         <f t="shared" ca="1" si="5"/>
-        <v>-154.05309657206334</v>
+        <v>-154.05309657336301</v>
       </c>
       <c r="R17">
         <f t="shared" ca="1" si="5"/>
-        <v>-160.14579612058586</v>
+        <v>-160.14579611253433</v>
       </c>
       <c r="S17">
         <f t="shared" ca="1" si="5"/>
-        <v>-166.59936710693592</v>
+        <v>-166.59936714534052</v>
       </c>
     </row>
     <row r="19" spans="1:19" s="8" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -4171,27 +4171,27 @@
       </c>
       <c r="N19" s="8">
         <f ca="1">+'P&amp;L'!N68</f>
-        <v>133.40042506941694</v>
+        <v>133.40042506941654</v>
       </c>
       <c r="O19" s="8">
         <f ca="1">+'P&amp;L'!O68</f>
-        <v>156.88120293542369</v>
+        <v>156.88120293542937</v>
       </c>
       <c r="P19" s="8">
         <f ca="1">+'P&amp;L'!P68</f>
-        <v>199.52909722433239</v>
+        <v>199.52909722427816</v>
       </c>
       <c r="Q19" s="8">
         <f ca="1">+'P&amp;L'!Q68</f>
-        <v>209.9476158804635</v>
+        <v>209.94761588085805</v>
       </c>
       <c r="R19" s="8">
         <f ca="1">+'P&amp;L'!R68</f>
-        <v>220.6921934042592</v>
+        <v>220.69219340191256</v>
       </c>
       <c r="S19" s="8">
         <f ca="1">+'P&amp;L'!S68</f>
-        <v>232.88019536965373</v>
+        <v>232.88019538282424</v>
       </c>
     </row>
     <row r="20" spans="1:19" s="2" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -4237,27 +4237,27 @@
       </c>
       <c r="N20" s="58">
         <f t="shared" ca="1" si="6"/>
-        <v>0.22610241537189313</v>
+        <v>0.22610241537189243</v>
       </c>
       <c r="O20" s="58">
         <f t="shared" ca="1" si="6"/>
-        <v>0.24322667121771113</v>
+        <v>0.24322667121771996</v>
       </c>
       <c r="P20" s="58">
         <f t="shared" ca="1" si="6"/>
-        <v>0.24041884738444277</v>
+        <v>0.24041884738437744</v>
       </c>
       <c r="Q20" s="58">
         <f t="shared" ca="1" si="6"/>
-        <v>0.24126240801041079</v>
+        <v>0.24126240801086418</v>
       </c>
       <c r="R20" s="58">
         <f t="shared" ca="1" si="6"/>
-        <v>0.24199367572259928</v>
+        <v>0.24199367572002611</v>
       </c>
       <c r="S20" s="58">
         <f t="shared" ca="1" si="6"/>
-        <v>0.24323157247624394</v>
+        <v>0.24323157248999988</v>
       </c>
     </row>
     <row r="22" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -4299,27 +4299,27 @@
       </c>
       <c r="N22" s="8">
         <f ca="1">+'P&amp;L'!N71</f>
-        <v>102.43140319177384</v>
+        <v>102.43140319177354</v>
       </c>
       <c r="O22" s="8">
         <f ca="1">+'P&amp;L'!O71</f>
-        <v>120.46109855142393</v>
+        <v>120.46109855142829</v>
       </c>
       <c r="P22" s="8">
         <f ca="1">+'P&amp;L'!P71</f>
-        <v>153.20824799202092</v>
+        <v>153.20824799197928</v>
       </c>
       <c r="Q22" s="8">
         <f ca="1">+'P&amp;L'!Q71</f>
-        <v>161.208098701431</v>
+        <v>161.20809870173397</v>
       </c>
       <c r="R22" s="8">
         <f ca="1">+'P&amp;L'!R71</f>
-        <v>169.45831343569805</v>
+        <v>169.45831343389617</v>
       </c>
       <c r="S22" s="8">
         <f ca="1">+'P&amp;L'!S71</f>
-        <v>178.81686040261977</v>
+        <v>178.81686041273272</v>
       </c>
     </row>
     <row r="24" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -4480,11 +4480,11 @@
   </sheetPr>
   <dimension ref="A1:T76"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView showGridLines="0" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane xSplit="4" ySplit="3" topLeftCell="F4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="F1" sqref="F1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="J6" sqref="J6"/>
+      <selection pane="bottomRight" activeCell="K21" sqref="K21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="15.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5269,31 +5269,31 @@
       </c>
       <c r="M22">
         <f ca="1">+IF(Circ=1, 'Debt Calcs'!M22, 0)</f>
-        <v>-46.609040079970399</v>
+        <v>-46.609040079970413</v>
       </c>
       <c r="N22">
         <f ca="1">+IF(Circ=1, 'Debt Calcs'!N22, 0)</f>
-        <v>-48.876198931842609</v>
+        <v>-48.876198931842218</v>
       </c>
       <c r="O22">
         <f ca="1">+IF(Circ=1, 'Debt Calcs'!O22, 0)</f>
-        <v>-51.074131365529389</v>
+        <v>-51.074131365534789</v>
       </c>
       <c r="P22">
         <f ca="1">+IF(Circ=1, 'Debt Calcs'!P22, 0)</f>
-        <v>-53.352727722206389</v>
+        <v>-53.352727722154505</v>
       </c>
       <c r="Q22">
         <f ca="1">+IF(Circ=1, 'Debt Calcs'!Q22, 0)</f>
-        <v>-54.877626088768707</v>
+        <v>-54.877626089172722</v>
       </c>
       <c r="R22">
         <f ca="1">+IF(Circ=1, 'Debt Calcs'!R22, 0)</f>
-        <v>-55.536109613090858</v>
+        <v>-55.536109610530367</v>
       </c>
       <c r="S22">
         <f ca="1">+IF(Circ=1, 'Debt Calcs'!S22, 0)</f>
-        <v>-55.952184566741735</v>
+        <v>-55.95218458028161</v>
       </c>
     </row>
     <row r="23" spans="2:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -5484,31 +5484,31 @@
       </c>
       <c r="M27" s="8">
         <f t="shared" ref="M27:S27" ca="1" si="4">+M13+SUM(M16:M18,M20:M25)</f>
-        <v>38.482799907115236</v>
+        <v>38.482799907115208</v>
       </c>
       <c r="N27" s="8">
         <f t="shared" ca="1" si="4"/>
-        <v>39.802833107753827</v>
+        <v>39.802833107754225</v>
       </c>
       <c r="O27" s="8">
         <f t="shared" ca="1" si="4"/>
-        <v>55.340476300034368</v>
+        <v>55.340476300028968</v>
       </c>
       <c r="P27" s="8">
         <f t="shared" ca="1" si="4"/>
-        <v>82.12671732238033</v>
+        <v>82.126717322432171</v>
       </c>
       <c r="Q27" s="8">
         <f t="shared" ca="1" si="4"/>
-        <v>88.847158755663372</v>
+        <v>88.847158755259329</v>
       </c>
       <c r="R27" s="8">
         <f t="shared" ca="1" si="4"/>
-        <v>95.532524960521926</v>
+        <v>95.532524963082437</v>
       </c>
       <c r="S27" s="8">
         <f t="shared" ca="1" si="4"/>
-        <v>103.42444219900585</v>
+        <v>103.42444218546598</v>
       </c>
     </row>
     <row r="28" spans="2:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -5549,31 +5549,31 @@
       </c>
       <c r="M28" s="48">
         <f t="shared" ref="M28:S28" ca="1" si="5">+M27/M6</f>
-        <v>6.8965591231389317E-2</v>
+        <v>6.8965591231389262E-2</v>
       </c>
       <c r="N28" s="48">
         <f t="shared" ca="1" si="5"/>
-        <v>6.7462428996192925E-2</v>
+        <v>6.7462428996193605E-2</v>
       </c>
       <c r="O28" s="48">
         <f t="shared" ca="1" si="5"/>
-        <v>8.5799188062068793E-2</v>
+        <v>8.5799188062060411E-2</v>
       </c>
       <c r="P28" s="48">
         <f t="shared" ca="1" si="5"/>
-        <v>9.8957049336595548E-2</v>
+        <v>9.8957049336658012E-2</v>
       </c>
       <c r="Q28" s="48">
         <f t="shared" ca="1" si="5"/>
-        <v>0.10209918019968932</v>
+        <v>0.10209918019922501</v>
       </c>
       <c r="R28" s="48">
         <f t="shared" ca="1" si="5"/>
-        <v>0.10475344193036371</v>
+        <v>0.10475344193317136</v>
       </c>
       <c r="S28" s="48">
         <f t="shared" ca="1" si="5"/>
-        <v>0.10802159311405596</v>
+        <v>0.10802159309991424</v>
       </c>
     </row>
     <row r="30" spans="2:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -5606,31 +5606,31 @@
       </c>
       <c r="M30" s="71">
         <f ca="1">+'FS Calcs'!M107</f>
-        <v>-11.160011973063392</v>
+        <v>-11.16001197306341</v>
       </c>
       <c r="N30" s="71">
         <f ca="1">+'FS Calcs'!N107</f>
-        <v>-11.542821601249154</v>
+        <v>-11.542821601248717</v>
       </c>
       <c r="O30" s="71">
         <f ca="1">+'FS Calcs'!O107</f>
-        <v>-16.04873812700281</v>
+        <v>-16.048738127008541</v>
       </c>
       <c r="P30" s="71">
         <f ca="1">+'FS Calcs'!P107</f>
-        <v>-23.816748023558031</v>
+        <v>-23.816748023503845</v>
       </c>
       <c r="Q30" s="71">
         <f ca="1">+'FS Calcs'!Q107</f>
-        <v>-25.765676038643125</v>
+        <v>-25.765676039037665</v>
       </c>
       <c r="R30" s="71">
         <f ca="1">+'FS Calcs'!R107</f>
-        <v>-27.704432241555477</v>
+        <v>-27.704432239208796</v>
       </c>
       <c r="S30" s="71">
         <f ca="1">+'FS Calcs'!S107</f>
-        <v>-29.99308822112625</v>
+        <v>-29.993088234296746</v>
       </c>
     </row>
     <row r="31" spans="2:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -5728,31 +5728,31 @@
       </c>
       <c r="M32">
         <f t="shared" ca="1" si="6"/>
-        <v>-11.160011973063392</v>
+        <v>-11.16001197306341</v>
       </c>
       <c r="N32">
         <f t="shared" ca="1" si="6"/>
-        <v>-11.542821601249154</v>
+        <v>-11.542821601248717</v>
       </c>
       <c r="O32">
         <f t="shared" ca="1" si="6"/>
-        <v>-16.04873812700281</v>
+        <v>-16.048738127008541</v>
       </c>
       <c r="P32">
         <f t="shared" ca="1" si="6"/>
-        <v>-23.816748023558031</v>
+        <v>-23.816748023503845</v>
       </c>
       <c r="Q32">
         <f t="shared" ca="1" si="6"/>
-        <v>-25.765676038643125</v>
+        <v>-25.765676039037665</v>
       </c>
       <c r="R32">
         <f t="shared" ca="1" si="6"/>
-        <v>-27.704432241555477</v>
+        <v>-27.704432239208796</v>
       </c>
       <c r="S32">
         <f t="shared" ca="1" si="6"/>
-        <v>-29.99308822112625</v>
+        <v>-29.993088234296746</v>
       </c>
     </row>
     <row r="34" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -5793,31 +5793,31 @@
       </c>
       <c r="M34">
         <f t="shared" ref="M34:S34" ca="1" si="7">+M32+M27</f>
-        <v>27.322787934051846</v>
+        <v>27.322787934051796</v>
       </c>
       <c r="N34">
         <f t="shared" ca="1" si="7"/>
-        <v>28.260011506504675</v>
+        <v>28.260011506505506</v>
       </c>
       <c r="O34">
         <f t="shared" ca="1" si="7"/>
-        <v>39.291738173031561</v>
+        <v>39.291738173020427</v>
       </c>
       <c r="P34">
         <f t="shared" ca="1" si="7"/>
-        <v>58.309969298822296</v>
+        <v>58.309969298928323</v>
       </c>
       <c r="Q34">
         <f t="shared" ca="1" si="7"/>
-        <v>63.081482717020251</v>
+        <v>63.081482716221664</v>
       </c>
       <c r="R34">
         <f t="shared" ca="1" si="7"/>
-        <v>67.828092718966445</v>
+        <v>67.828092723873638</v>
       </c>
       <c r="S34">
         <f t="shared" ca="1" si="7"/>
-        <v>73.43135397787961</v>
+        <v>73.431353951169228</v>
       </c>
     </row>
     <row r="35" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -5915,31 +5915,31 @@
       </c>
       <c r="M36" s="8">
         <f t="shared" ref="M36:S36" ca="1" si="8">+M34-M35</f>
-        <v>-2.0707570380051976</v>
+        <v>-2.0707570380052474</v>
       </c>
       <c r="N36" s="8">
         <f t="shared" ca="1" si="8"/>
-        <v>-2.0153398147140855</v>
+        <v>-2.0153398147132542</v>
       </c>
       <c r="O36" s="8">
         <f t="shared" ca="1" si="8"/>
-        <v>8.1081263121762355</v>
+        <v>8.1081263121651013</v>
       </c>
       <c r="P36" s="8">
         <f t="shared" ca="1" si="8"/>
-        <v>26.190849082141305</v>
+        <v>26.190849082247333</v>
       </c>
       <c r="Q36" s="8">
         <f t="shared" ca="1" si="8"/>
-        <v>29.998788893838842</v>
+        <v>29.998788893040256</v>
       </c>
       <c r="R36" s="8">
         <f t="shared" ca="1" si="8"/>
-        <v>33.752918081089575</v>
+        <v>33.752918085996768</v>
       </c>
       <c r="S36" s="8">
         <f t="shared" ca="1" si="8"/>
-        <v>38.333924100866447</v>
+        <v>38.333924074156066</v>
       </c>
     </row>
     <row r="38" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -5975,31 +5975,31 @@
       </c>
       <c r="M38" s="45">
         <f t="shared" ref="M38:S39" ca="1" si="9">+M$36/M41</f>
-        <v>-1.1962778960168676E-2</v>
+        <v>-1.1962778960168962E-2</v>
       </c>
       <c r="N38" s="45">
         <f t="shared" ca="1" si="9"/>
-        <v>-1.1642633245026492E-2</v>
+        <v>-1.1642633245021688E-2</v>
       </c>
       <c r="O38" s="45">
         <f t="shared" ca="1" si="9"/>
-        <v>4.684070659836069E-2</v>
+        <v>4.6840706598296367E-2</v>
       </c>
       <c r="P38" s="45">
         <f t="shared" ca="1" si="9"/>
-        <v>0.15130473184368173</v>
+        <v>0.15130473184429424</v>
       </c>
       <c r="Q38" s="45">
         <f t="shared" ca="1" si="9"/>
-        <v>0.17330322873390436</v>
+        <v>0.17330322872929091</v>
       </c>
       <c r="R38" s="45">
         <f t="shared" ca="1" si="9"/>
-        <v>0.19499086124257409</v>
+        <v>0.19499086127092299</v>
       </c>
       <c r="S38" s="45">
         <f t="shared" ca="1" si="9"/>
-        <v>0.22145536742268312</v>
+        <v>0.22145536726837706</v>
       </c>
     </row>
     <row r="39" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -6035,31 +6035,31 @@
       </c>
       <c r="M39" s="45">
         <f t="shared" ca="1" si="9"/>
-        <v>-1.0875824779439063E-2</v>
+        <v>-1.0875824779439325E-2</v>
       </c>
       <c r="N39" s="45">
         <f t="shared" ca="1" si="9"/>
-        <v>-1.0584767934422718E-2</v>
+        <v>-1.0584767934418352E-2</v>
       </c>
       <c r="O39" s="45">
         <f t="shared" ca="1" si="9"/>
-        <v>4.2584697017732327E-2</v>
+        <v>4.2584697017673853E-2</v>
       </c>
       <c r="P39" s="45">
         <f t="shared" ca="1" si="9"/>
-        <v>0.13755698047343123</v>
+        <v>0.13755698047398809</v>
       </c>
       <c r="Q39" s="45">
         <f t="shared" ca="1" si="9"/>
-        <v>0.15755666435839727</v>
+        <v>0.15755666435420301</v>
       </c>
       <c r="R39" s="45">
         <f t="shared" ca="1" si="9"/>
-        <v>0.17727372941748726</v>
+        <v>0.17727372944326034</v>
       </c>
       <c r="S39" s="45">
         <f t="shared" ca="1" si="9"/>
-        <v>0.20133363498354226</v>
+        <v>0.20133363484325664</v>
       </c>
     </row>
     <row r="41" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -6349,31 +6349,31 @@
       </c>
       <c r="M48">
         <f t="shared" ca="1" si="11"/>
-        <v>38.482799907115236</v>
+        <v>38.482799907115208</v>
       </c>
       <c r="N48">
         <f t="shared" ca="1" si="11"/>
-        <v>39.802833107753827</v>
+        <v>39.802833107754225</v>
       </c>
       <c r="O48">
         <f t="shared" ca="1" si="11"/>
-        <v>55.340476300034368</v>
+        <v>55.340476300028968</v>
       </c>
       <c r="P48">
         <f t="shared" ca="1" si="11"/>
-        <v>82.12671732238033</v>
+        <v>82.126717322432171</v>
       </c>
       <c r="Q48">
         <f t="shared" ca="1" si="11"/>
-        <v>88.847158755663372</v>
+        <v>88.847158755259329</v>
       </c>
       <c r="R48">
         <f t="shared" ca="1" si="11"/>
-        <v>95.532524960521926</v>
+        <v>95.532524963082437</v>
       </c>
       <c r="S48">
         <f t="shared" ca="1" si="11"/>
-        <v>103.42444219900585</v>
+        <v>103.42444218546598</v>
       </c>
     </row>
     <row r="49" spans="2:20" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -6414,31 +6414,31 @@
       </c>
       <c r="M49">
         <f t="shared" ca="1" si="12"/>
-        <v>11.160011973063392</v>
+        <v>11.16001197306341</v>
       </c>
       <c r="N49">
         <f t="shared" ca="1" si="12"/>
-        <v>11.542821601249154</v>
+        <v>11.542821601248717</v>
       </c>
       <c r="O49">
         <f t="shared" ca="1" si="12"/>
-        <v>16.04873812700281</v>
+        <v>16.048738127008541</v>
       </c>
       <c r="P49">
         <f t="shared" ca="1" si="12"/>
-        <v>23.816748023558031</v>
+        <v>23.816748023503845</v>
       </c>
       <c r="Q49">
         <f t="shared" ca="1" si="12"/>
-        <v>25.765676038643125</v>
+        <v>25.765676039037665</v>
       </c>
       <c r="R49">
         <f t="shared" ca="1" si="12"/>
-        <v>27.704432241555477</v>
+        <v>27.704432239208796</v>
       </c>
       <c r="S49">
         <f t="shared" ca="1" si="12"/>
-        <v>29.99308822112625</v>
+        <v>29.993088234296746</v>
       </c>
     </row>
     <row r="50" spans="2:20" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -6479,31 +6479,31 @@
       </c>
       <c r="M50">
         <f t="shared" ca="1" si="13"/>
-        <v>46.609040079970399</v>
+        <v>46.609040079970413</v>
       </c>
       <c r="N50">
         <f t="shared" ca="1" si="13"/>
-        <v>48.876198931842609</v>
+        <v>48.876198931842218</v>
       </c>
       <c r="O50">
         <f t="shared" ca="1" si="13"/>
-        <v>51.074131365529389</v>
+        <v>51.074131365534789</v>
       </c>
       <c r="P50">
         <f t="shared" ca="1" si="13"/>
-        <v>53.352727722206389</v>
+        <v>53.352727722154505</v>
       </c>
       <c r="Q50">
         <f t="shared" ca="1" si="13"/>
-        <v>54.877626088768707</v>
+        <v>54.877626089172722</v>
       </c>
       <c r="R50">
         <f t="shared" ca="1" si="13"/>
-        <v>55.536109613090858</v>
+        <v>55.536109610530367</v>
       </c>
       <c r="S50">
         <f t="shared" ca="1" si="13"/>
-        <v>55.952184566741735</v>
+        <v>55.95218458028161</v>
       </c>
     </row>
     <row r="51" spans="2:20" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -6875,27 +6875,27 @@
       </c>
       <c r="N56" s="54">
         <f t="shared" ca="1" si="19"/>
-        <v>145.90042506941694</v>
+        <v>145.90042506941654</v>
       </c>
       <c r="O56" s="54">
         <f t="shared" ca="1" si="19"/>
-        <v>169.38120293542369</v>
+        <v>169.38120293542937</v>
       </c>
       <c r="P56" s="54">
         <f t="shared" ca="1" si="19"/>
-        <v>212.02909722433239</v>
+        <v>212.02909722427816</v>
       </c>
       <c r="Q56" s="54">
         <f t="shared" ca="1" si="19"/>
-        <v>222.4476158804635</v>
+        <v>222.44761588085805</v>
       </c>
       <c r="R56" s="54">
         <f t="shared" ca="1" si="19"/>
-        <v>233.1921934042592</v>
+        <v>233.19219340191256</v>
       </c>
       <c r="S56" s="54">
         <f t="shared" ca="1" si="19"/>
-        <v>245.38019536965373</v>
+        <v>245.38019538282424</v>
       </c>
     </row>
     <row r="57" spans="2:20" s="2" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -6940,27 +6940,27 @@
       </c>
       <c r="N57" s="58">
         <f t="shared" ca="1" si="20"/>
-        <v>0.24728885604985923</v>
+        <v>0.24728885604985854</v>
       </c>
       <c r="O57" s="58">
         <f t="shared" ca="1" si="20"/>
-        <v>0.26260651617895148</v>
+        <v>0.26260651617896025</v>
       </c>
       <c r="P57" s="58">
         <f t="shared" ca="1" si="20"/>
-        <v>0.25548048818827362</v>
+        <v>0.25548048818820829</v>
       </c>
       <c r="Q57" s="58">
         <f t="shared" ca="1" si="20"/>
-        <v>0.25562684881381204</v>
+        <v>0.25562684881426539</v>
       </c>
       <c r="R57" s="58">
         <f t="shared" ca="1" si="20"/>
-        <v>0.25570019111796488</v>
+        <v>0.25570019111539177</v>
       </c>
       <c r="S57" s="58">
         <f t="shared" ca="1" si="20"/>
-        <v>0.25628718955491819</v>
+        <v>0.25628718956867413</v>
       </c>
     </row>
     <row r="58" spans="2:20" s="8" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -7001,27 +7001,27 @@
       </c>
       <c r="N59" s="8">
         <f t="shared" ca="1" si="21"/>
-        <v>-33.870907484597481</v>
+        <v>-33.870907484597389</v>
       </c>
       <c r="O59" s="8">
         <f t="shared" ca="1" si="21"/>
-        <v>-39.321989990954137</v>
+        <v>-39.321989990955451</v>
       </c>
       <c r="P59" s="8">
         <f t="shared" ca="1" si="21"/>
-        <v>-49.222734839265854</v>
+        <v>-49.222734839253263</v>
       </c>
       <c r="Q59" s="8">
         <f t="shared" ca="1" si="21"/>
-        <v>-51.64140278598687</v>
+        <v>-51.641402786078466</v>
       </c>
       <c r="R59" s="8">
         <f t="shared" ca="1" si="21"/>
-        <v>-54.135765575515542</v>
+        <v>-54.135765574970762</v>
       </c>
       <c r="S59" s="8">
         <f t="shared" ca="1" si="21"/>
-        <v>-56.965220573988354</v>
+        <v>-56.965220577045898</v>
       </c>
     </row>
     <row r="60" spans="2:20" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -7152,27 +7152,27 @@
       </c>
       <c r="N62" s="80">
         <f t="shared" ca="1" si="23"/>
-        <v>112.02951758481946</v>
+        <v>112.02951758481916</v>
       </c>
       <c r="O62" s="80">
         <f t="shared" ca="1" si="23"/>
-        <v>130.05921294446955</v>
+        <v>130.05921294447393</v>
       </c>
       <c r="P62" s="80">
         <f t="shared" ca="1" si="23"/>
-        <v>162.80636238506654</v>
+        <v>162.8063623850249</v>
       </c>
       <c r="Q62" s="80">
         <f t="shared" ca="1" si="23"/>
-        <v>170.80621309447662</v>
+        <v>170.80621309477959</v>
       </c>
       <c r="R62" s="80">
         <f t="shared" ca="1" si="23"/>
-        <v>179.05642782874367</v>
+        <v>179.05642782694179</v>
       </c>
       <c r="S62" s="80">
         <f t="shared" ca="1" si="23"/>
-        <v>188.41497479566539</v>
+        <v>188.41497480577834</v>
       </c>
       <c r="T62" s="81"/>
     </row>
@@ -7218,27 +7218,27 @@
       </c>
       <c r="N63" s="58">
         <f t="shared" ca="1" si="24"/>
-        <v>0.18988053827935503</v>
+        <v>0.1898805382793545</v>
       </c>
       <c r="O63" s="58">
         <f t="shared" ca="1" si="24"/>
-        <v>0.2016421906115807</v>
+        <v>0.20164219061158747</v>
       </c>
       <c r="P63" s="58">
         <f t="shared" ca="1" si="24"/>
-        <v>0.19617047606577503</v>
+        <v>0.19617047606572485</v>
       </c>
       <c r="Q63" s="58">
         <f t="shared" ca="1" si="24"/>
-        <v>0.19628285894789943</v>
+        <v>0.1962828589482476</v>
       </c>
       <c r="R63" s="58">
         <f t="shared" ca="1" si="24"/>
-        <v>0.19633917477390819</v>
+        <v>0.19633917477193238</v>
       </c>
       <c r="S63" s="58">
         <f t="shared" ca="1" si="24"/>
-        <v>0.19678990102562152</v>
+        <v>0.19678990103618399</v>
       </c>
     </row>
     <row r="64" spans="2:20" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -7483,27 +7483,27 @@
       </c>
       <c r="N68" s="54">
         <f t="shared" ca="1" si="28"/>
-        <v>133.40042506941694</v>
+        <v>133.40042506941654</v>
       </c>
       <c r="O68" s="54">
         <f t="shared" ca="1" si="28"/>
-        <v>156.88120293542369</v>
+        <v>156.88120293542937</v>
       </c>
       <c r="P68" s="54">
         <f t="shared" ca="1" si="28"/>
-        <v>199.52909722433239</v>
+        <v>199.52909722427816</v>
       </c>
       <c r="Q68" s="54">
         <f t="shared" ca="1" si="28"/>
-        <v>209.9476158804635</v>
+        <v>209.94761588085805</v>
       </c>
       <c r="R68" s="54">
         <f t="shared" ca="1" si="28"/>
-        <v>220.6921934042592</v>
+        <v>220.69219340191256</v>
       </c>
       <c r="S68" s="54">
         <f t="shared" ca="1" si="28"/>
-        <v>232.88019536965373</v>
+        <v>232.88019538282424</v>
       </c>
     </row>
     <row r="69" spans="2:19" s="8" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -7548,27 +7548,27 @@
       </c>
       <c r="N69" s="58">
         <f t="shared" ca="1" si="29"/>
-        <v>0.22610241537189313</v>
+        <v>0.22610241537189243</v>
       </c>
       <c r="O69" s="58">
         <f t="shared" ca="1" si="29"/>
-        <v>0.24322667121771113</v>
+        <v>0.24322667121771996</v>
       </c>
       <c r="P69" s="58">
         <f t="shared" ca="1" si="29"/>
-        <v>0.24041884738444277</v>
+        <v>0.24041884738437744</v>
       </c>
       <c r="Q69" s="58">
         <f t="shared" ca="1" si="29"/>
-        <v>0.24126240801041079</v>
+        <v>0.24126240801086418</v>
       </c>
       <c r="R69" s="58">
         <f t="shared" ca="1" si="29"/>
-        <v>0.24199367572259928</v>
+        <v>0.24199367572002611</v>
       </c>
       <c r="S69" s="58">
         <f t="shared" ca="1" si="29"/>
-        <v>0.24323157247624394</v>
+        <v>0.24323157248999988</v>
       </c>
     </row>
     <row r="70" spans="2:19" s="8" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -7616,27 +7616,27 @@
       </c>
       <c r="N71" s="80">
         <f t="shared" ca="1" si="30"/>
-        <v>102.43140319177384</v>
+        <v>102.43140319177354</v>
       </c>
       <c r="O71" s="80">
         <f t="shared" ca="1" si="30"/>
-        <v>120.46109855142393</v>
+        <v>120.46109855142829</v>
       </c>
       <c r="P71" s="80">
         <f t="shared" ca="1" si="30"/>
-        <v>153.20824799202092</v>
+        <v>153.20824799197928</v>
       </c>
       <c r="Q71" s="80">
         <f t="shared" ca="1" si="30"/>
-        <v>161.208098701431</v>
+        <v>161.20809870173397</v>
       </c>
       <c r="R71" s="80">
         <f t="shared" ca="1" si="30"/>
-        <v>169.45831343569805</v>
+        <v>169.45831343389617</v>
       </c>
       <c r="S71" s="80">
         <f t="shared" ca="1" si="30"/>
-        <v>178.81686040261977</v>
+        <v>178.81686041273272</v>
       </c>
     </row>
     <row r="72" spans="2:19" s="2" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -7681,27 +7681,27 @@
       </c>
       <c r="N72" s="58">
         <f t="shared" ca="1" si="31"/>
-        <v>0.17361254778266752</v>
+        <v>0.17361254778266702</v>
       </c>
       <c r="O72" s="58">
         <f t="shared" ca="1" si="31"/>
-        <v>0.18676139310298284</v>
+        <v>0.18676139310298961</v>
       </c>
       <c r="P72" s="58">
         <f t="shared" ca="1" si="31"/>
-        <v>0.18460540795520447</v>
+        <v>0.18460540795515432</v>
       </c>
       <c r="Q72" s="58">
         <f t="shared" ca="1" si="31"/>
-        <v>0.18525313526604528</v>
+        <v>0.18525313526639345</v>
       </c>
       <c r="R72" s="58">
         <f t="shared" ca="1" si="31"/>
-        <v>0.18581463855832736</v>
+        <v>0.18581463855635155</v>
       </c>
       <c r="S72" s="58">
         <f t="shared" ca="1" si="31"/>
-        <v>0.18676515653018827</v>
+        <v>0.18676515654075074</v>
       </c>
     </row>
     <row r="74" spans="2:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -7865,11 +7865,11 @@
   </sheetPr>
   <dimension ref="A1:S122"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane xSplit="4" ySplit="3" topLeftCell="F4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="F1" sqref="F1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="J57" sqref="J57"/>
+      <selection pane="bottomRight" activeCell="K5" sqref="K5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="15.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9142,31 +9142,31 @@
       </c>
       <c r="M29" s="71">
         <f ca="1">+'Debt Calcs'!M13</f>
-        <v>719.67975458408853</v>
+        <v>719.67975458408625</v>
       </c>
       <c r="N29" s="71">
         <f ca="1">+'Debt Calcs'!N13</f>
-        <v>757.44874298165223</v>
+        <v>757.44874298170851</v>
       </c>
       <c r="O29" s="71">
         <f ca="1">+'Debt Calcs'!O13</f>
-        <v>798.17734150242086</v>
+        <v>798.17734150165973</v>
       </c>
       <c r="P29" s="71">
         <f ca="1">+'Debt Calcs'!P13</f>
-        <v>838.8271842823209</v>
+        <v>838.82718428975647</v>
       </c>
       <c r="Q29" s="71">
         <f ca="1">+'Debt Calcs'!Q13</f>
-        <v>852.63799752090347</v>
+        <v>852.63799746487859</v>
       </c>
       <c r="R29" s="71">
         <f ca="1">+'Debt Calcs'!R13</f>
-        <v>862.34445257666266</v>
+        <v>862.34445292168812</v>
       </c>
       <c r="S29" s="71">
         <f ca="1">+'Debt Calcs'!S13</f>
-        <v>867.49781970665595</v>
+        <v>867.49781773964776</v>
       </c>
     </row>
     <row r="30" spans="2:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -9378,31 +9378,31 @@
       </c>
       <c r="M33" s="8">
         <f t="shared" ref="M33:S33" ca="1" si="8">+SUM(M29:M32,M27)</f>
-        <v>1176.1799548837434</v>
+        <v>1176.1799548837412</v>
       </c>
       <c r="N33" s="8">
         <f t="shared" ca="1" si="8"/>
-        <v>1230.958413214305</v>
+        <v>1230.9584132143611</v>
       </c>
       <c r="O33" s="8">
         <f t="shared" ca="1" si="8"/>
-        <v>1293.3086176889631</v>
+        <v>1293.3086176882018</v>
       </c>
       <c r="P33" s="8">
         <f t="shared" ca="1" si="8"/>
-        <v>1424.973829488064</v>
+        <v>1424.9738294954996</v>
       </c>
       <c r="Q33" s="8">
         <f t="shared" ca="1" si="8"/>
-        <v>1458.0582200339986</v>
+        <v>1458.0582199779737</v>
       </c>
       <c r="R33" s="8">
         <f t="shared" ca="1" si="8"/>
-        <v>1487.7360581987768</v>
+        <v>1487.7360585438023</v>
       </c>
       <c r="S33" s="8">
         <f t="shared" ca="1" si="8"/>
-        <v>1514.4291961893211</v>
+        <v>1514.4291942223131</v>
       </c>
     </row>
     <row r="35" spans="2:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -9438,31 +9438,31 @@
       </c>
       <c r="M35" s="68">
         <f t="shared" ca="1" si="9"/>
-        <v>-48.556757038007561</v>
+        <v>-48.556757038005287</v>
       </c>
       <c r="N35" s="68">
         <f t="shared" ca="1" si="9"/>
-        <v>-50.572096852663464</v>
+        <v>-50.572096852719625</v>
       </c>
       <c r="O35" s="68">
         <f t="shared" ca="1" si="9"/>
-        <v>-42.4639705413</v>
+        <v>-42.463970540538753</v>
       </c>
       <c r="P35" s="71">
         <f ca="1">+'FS Calcs'!P78</f>
-        <v>119.54087853967529</v>
+        <v>119.54087854173562</v>
       </c>
       <c r="Q35" s="71">
         <f ca="1">+'FS Calcs'!Q78</f>
-        <v>149.53966745085461</v>
+        <v>149.53966743436553</v>
       </c>
       <c r="R35" s="71">
         <f ca="1">+'FS Calcs'!R78</f>
-        <v>183.29258541551306</v>
+        <v>183.29258552344811</v>
       </c>
       <c r="S35" s="71">
         <f ca="1">+'FS Calcs'!S78</f>
-        <v>221.62651016955888</v>
+        <v>221.62650957805627</v>
       </c>
     </row>
     <row r="36" spans="2:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -9560,31 +9560,31 @@
       </c>
       <c r="M37" s="8">
         <f t="shared" ref="M37:S37" ca="1" si="10">+M36+M35</f>
-        <v>160.51820219660954</v>
+        <v>160.51820219661181</v>
       </c>
       <c r="N37" s="8">
         <f t="shared" ca="1" si="10"/>
-        <v>151.67116198842359</v>
+        <v>151.67116198836743</v>
       </c>
       <c r="O37" s="8">
         <f t="shared" ca="1" si="10"/>
-        <v>153.11370741159863</v>
+        <v>153.11370741235987</v>
       </c>
       <c r="P37" s="8">
         <f t="shared" ca="1" si="10"/>
-        <v>308.63150010523026</v>
+        <v>308.63150010729055</v>
       </c>
       <c r="Q37" s="8">
         <f t="shared" ca="1" si="10"/>
-        <v>332.33468270348584</v>
+        <v>332.33468268699676</v>
       </c>
       <c r="R37" s="8">
         <f t="shared" ca="1" si="10"/>
-        <v>359.99690916719396</v>
+        <v>359.99690927512898</v>
       </c>
       <c r="S37" s="8">
         <f t="shared" ca="1" si="10"/>
-        <v>392.45908033664909</v>
+        <v>392.45907974514648</v>
       </c>
     </row>
     <row r="39" spans="2:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -10016,31 +10016,31 @@
       </c>
       <c r="M47" s="8">
         <f t="shared" ref="M47:S47" ca="1" si="16">+M21+M26+M29+M24</f>
-        <v>850.17975458408853</v>
+        <v>850.17975458408625</v>
       </c>
       <c r="N47" s="8">
         <f t="shared" ca="1" si="16"/>
-        <v>887.94874298165223</v>
+        <v>887.94874298170851</v>
       </c>
       <c r="O47" s="8">
         <f t="shared" ca="1" si="16"/>
-        <v>928.67734150242086</v>
+        <v>928.67734150165973</v>
       </c>
       <c r="P47" s="8">
         <f t="shared" ca="1" si="16"/>
-        <v>969.3271842823209</v>
+        <v>969.32718428975647</v>
       </c>
       <c r="Q47" s="8">
         <f t="shared" ca="1" si="16"/>
-        <v>983.13799752090347</v>
+        <v>983.13799746487859</v>
       </c>
       <c r="R47" s="8">
         <f t="shared" ca="1" si="16"/>
-        <v>992.84445257666266</v>
+        <v>992.84445292168812</v>
       </c>
       <c r="S47" s="8">
         <f t="shared" ca="1" si="16"/>
-        <v>997.99781970665595</v>
+        <v>997.99781773964776</v>
       </c>
     </row>
     <row r="48" spans="2:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -10083,31 +10083,31 @@
       </c>
       <c r="M48" s="8">
         <f t="shared" ref="M48:S48" ca="1" si="17">+M47+M25+M30</f>
-        <v>886.41875458408856</v>
+        <v>886.41875458408629</v>
       </c>
       <c r="N48" s="8">
         <f t="shared" ca="1" si="17"/>
-        <v>924.18774298165226</v>
+        <v>924.18774298170854</v>
       </c>
       <c r="O48" s="8">
         <f t="shared" ca="1" si="17"/>
-        <v>964.91634150242089</v>
+        <v>964.91634150165976</v>
       </c>
       <c r="P48" s="8">
         <f t="shared" ca="1" si="17"/>
-        <v>1005.5661842823209</v>
+        <v>1005.5661842897565</v>
       </c>
       <c r="Q48" s="8">
         <f t="shared" ca="1" si="17"/>
-        <v>1019.3769975209035</v>
+        <v>1019.3769974648786</v>
       </c>
       <c r="R48" s="8">
         <f t="shared" ca="1" si="17"/>
-        <v>1029.0834525766627</v>
+        <v>1029.0834529216881</v>
       </c>
       <c r="S48" s="8">
         <f t="shared" ca="1" si="17"/>
-        <v>1034.236819706656</v>
+        <v>1034.2368177396477</v>
       </c>
     </row>
     <row r="49" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -10170,31 +10170,31 @@
       </c>
       <c r="M50" s="8">
         <f t="shared" ref="M50:S50" ca="1" si="18">+M48-M44</f>
-        <v>851.41875458408856</v>
+        <v>851.41875458408629</v>
       </c>
       <c r="N50" s="8">
         <f t="shared" ca="1" si="18"/>
-        <v>889.18774298165226</v>
+        <v>889.18774298170854</v>
       </c>
       <c r="O50" s="8">
         <f t="shared" ca="1" si="18"/>
-        <v>929.91634150242089</v>
+        <v>929.91634150165976</v>
       </c>
       <c r="P50" s="8">
         <f t="shared" ca="1" si="18"/>
-        <v>970.56618428232093</v>
+        <v>970.56618428975651</v>
       </c>
       <c r="Q50" s="8">
         <f t="shared" ca="1" si="18"/>
-        <v>984.3769975209035</v>
+        <v>984.37699746487863</v>
       </c>
       <c r="R50" s="8">
         <f t="shared" ca="1" si="18"/>
-        <v>994.08345257666269</v>
+        <v>994.08345292168815</v>
       </c>
       <c r="S50" s="8">
         <f t="shared" ca="1" si="18"/>
-        <v>999.23681970665598</v>
+        <v>999.23681773964768</v>
       </c>
     </row>
     <row r="51" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -10257,31 +10257,31 @@
       </c>
       <c r="M52" s="84">
         <f ca="1">+M50/'P&amp;L'!M56</f>
-        <v>6.0183516397956298</v>
+        <v>6.0183516397956165</v>
       </c>
       <c r="N52" s="84">
         <f ca="1">+N50/'P&amp;L'!N56</f>
-        <v>6.0944835668477619</v>
+        <v>6.0944835668480764</v>
       </c>
       <c r="O52" s="84">
         <f ca="1">+O50/'P&amp;L'!O56</f>
-        <v>5.4900799226039521</v>
+        <v>5.4900799226001507</v>
       </c>
       <c r="P52" s="84">
         <f ca="1">+P50/'P&amp;L'!P56</f>
-        <v>4.5775141100399201</v>
+        <v>4.5775141100709185</v>
       </c>
       <c r="Q52" s="84">
         <f ca="1">+Q50/'P&amp;L'!Q56</f>
-        <v>4.4252081264946801</v>
+        <v>4.4252081262686787</v>
       </c>
       <c r="R52" s="84">
         <f ca="1">+R50/'P&amp;L'!R56</f>
-        <v>4.2629362420226435</v>
+        <v>4.2629362433550311</v>
       </c>
       <c r="S52" s="84">
         <f ca="1">+S50/'P&amp;L'!S56</f>
-        <v>4.0721983206429337</v>
+        <v>4.0721983132641109</v>
       </c>
     </row>
     <row r="53" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -10335,31 +10335,31 @@
       </c>
       <c r="M56" s="71">
         <f ca="1">+'P&amp;L'!M34</f>
-        <v>27.322787934051668</v>
+        <v>27.322787934051796</v>
       </c>
       <c r="N56" s="71">
         <f ca="1">+'P&amp;L'!N34</f>
-        <v>28.260011506508626</v>
+        <v>28.260011506505439</v>
       </c>
       <c r="O56" s="71">
         <f ca="1">+'P&amp;L'!O34</f>
-        <v>39.291738172980317</v>
+        <v>39.291738173021443</v>
       </c>
       <c r="P56" s="71">
         <f ca="1">+'P&amp;L'!P34</f>
-        <v>58.309969299293215</v>
+        <v>58.309969298917849</v>
       </c>
       <c r="Q56" s="71">
         <f ca="1">+'P&amp;L'!Q34</f>
-        <v>63.081482713646949</v>
+        <v>63.081482716307121</v>
       </c>
       <c r="R56" s="71">
         <f ca="1">+'P&amp;L'!R34</f>
-        <v>67.828092739437665</v>
+        <v>67.828092723294134</v>
       </c>
       <c r="S56" s="71">
         <f ca="1">+'P&amp;L'!S34</f>
-        <v>73.431353870760319</v>
+        <v>73.431353954580459</v>
       </c>
     </row>
     <row r="57" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -10678,31 +10678,31 @@
       </c>
       <c r="M63" s="71">
         <f ca="1">+'P&amp;L'!M22*-1</f>
-        <v>46.609040079970477</v>
+        <v>46.609040079970413</v>
       </c>
       <c r="N63" s="71">
         <f ca="1">+'P&amp;L'!N22*-1</f>
-        <v>48.87619893184074</v>
+        <v>48.876198931842247</v>
       </c>
       <c r="O63" s="71">
         <f ca="1">+'P&amp;L'!O22*-1</f>
-        <v>51.074131365554045</v>
+        <v>51.074131365534306</v>
       </c>
       <c r="P63" s="71">
         <f ca="1">+'P&amp;L'!P22*-1</f>
-        <v>53.352727721972769</v>
+        <v>53.352727722159649</v>
       </c>
       <c r="Q63" s="71">
         <f ca="1">+'P&amp;L'!Q22*-1</f>
-        <v>54.877626090490274</v>
+        <v>54.877626089129777</v>
       </c>
       <c r="R63" s="71">
         <f ca="1">+'P&amp;L'!R22*-1</f>
-        <v>55.536109602731841</v>
+        <v>55.536109610823857</v>
       </c>
       <c r="S63" s="71">
         <f ca="1">+'P&amp;L'!S22*-1</f>
-        <v>55.952184623932915</v>
+        <v>55.952184578517404</v>
       </c>
     </row>
     <row r="64" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -10772,31 +10772,31 @@
       </c>
       <c r="M65" s="54">
         <f t="shared" ca="1" si="20"/>
-        <v>70.477531947609776</v>
+        <v>70.477531947609847</v>
       </c>
       <c r="N65" s="54">
         <f t="shared" ca="1" si="20"/>
-        <v>80.664262248971482</v>
+        <v>80.664262248969806</v>
       </c>
       <c r="O65" s="54">
         <f t="shared" ca="1" si="20"/>
-        <v>83.669725594590716</v>
+        <v>83.669725594612089</v>
       </c>
       <c r="P65" s="54">
         <f t="shared" ca="1" si="20"/>
-        <v>96.954818793861406</v>
+        <v>96.954818793672928</v>
       </c>
       <c r="Q65" s="54">
         <f t="shared" ca="1" si="20"/>
-        <v>128.30635661469557</v>
+        <v>128.30635661599524</v>
       </c>
       <c r="R65" s="54">
         <f t="shared" ca="1" si="20"/>
-        <v>136.15414780832407</v>
+        <v>136.15414780027254</v>
       </c>
       <c r="S65" s="54">
         <f t="shared" ca="1" si="20"/>
-        <v>144.42732943506977</v>
+        <v>144.4273294734744</v>
       </c>
     </row>
     <row r="66" spans="2:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -11068,31 +11068,31 @@
       </c>
       <c r="M73" s="71">
         <f ca="1">+'Debt Calcs'!M39+'Debt Calcs'!M45+'Debt Calcs'!M51+'Debt Calcs'!M56</f>
-        <v>43.20097059780003</v>
+        <v>43.200970597800584</v>
       </c>
       <c r="N73" s="71">
         <f ca="1">+'Debt Calcs'!N39+'Debt Calcs'!N45+'Debt Calcs'!N51+'Debt Calcs'!N56</f>
-        <v>37.768988397633294</v>
+        <v>37.768988397620959</v>
       </c>
       <c r="O73" s="71">
         <f ca="1">+'Debt Calcs'!O39+'Debt Calcs'!O45+'Debt Calcs'!O51+'Debt Calcs'!O56</f>
-        <v>40.72859851981881</v>
+        <v>40.728598519969765</v>
       </c>
       <c r="P73" s="71">
         <f ca="1">+'Debt Calcs'!P39+'Debt Calcs'!P45+'Debt Calcs'!P51+'Debt Calcs'!P56</f>
-        <v>40.649842789193748</v>
+        <v>40.649842787894571</v>
       </c>
       <c r="Q73" s="71">
         <f ca="1">+'Debt Calcs'!Q39+'Debt Calcs'!Q45+'Debt Calcs'!Q51+'Debt Calcs'!Q56</f>
-        <v>13.810813167804367</v>
+        <v>13.810813176857847</v>
       </c>
       <c r="R73" s="71">
         <f ca="1">+'Debt Calcs'!R39+'Debt Calcs'!R45+'Debt Calcs'!R51+'Debt Calcs'!R56</f>
-        <v>9.706455496502107</v>
+        <v>9.706455444591759</v>
       </c>
       <c r="S73" s="71">
         <f ca="1">+'Debt Calcs'!S39+'Debt Calcs'!S45+'Debt Calcs'!S51+'Debt Calcs'!S56</f>
-        <v>5.1533646467081535</v>
+        <v>5.1533648931852252</v>
       </c>
     </row>
     <row r="74" spans="2:19" s="8" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -11264,31 +11264,31 @@
       </c>
       <c r="M77" s="71">
         <f ca="1">+'P&amp;L'!M22</f>
-        <v>-46.609040079970477</v>
+        <v>-46.609040079970413</v>
       </c>
       <c r="N77" s="71">
         <f ca="1">+'P&amp;L'!N22</f>
-        <v>-48.87619893184074</v>
+        <v>-48.876198931842247</v>
       </c>
       <c r="O77" s="71">
         <f ca="1">+'P&amp;L'!O22</f>
-        <v>-51.074131365554045</v>
+        <v>-51.074131365534306</v>
       </c>
       <c r="P77" s="71">
         <f ca="1">+'P&amp;L'!P22</f>
-        <v>-53.352727721972769</v>
+        <v>-53.352727722159649</v>
       </c>
       <c r="Q77" s="71">
         <f ca="1">+'P&amp;L'!Q22</f>
-        <v>-54.877626090490274</v>
+        <v>-54.877626089129777</v>
       </c>
       <c r="R77" s="71">
         <f ca="1">+'P&amp;L'!R22</f>
-        <v>-55.536109602731841</v>
+        <v>-55.536109610823857</v>
       </c>
       <c r="S77" s="71">
         <f ca="1">+'P&amp;L'!S22</f>
-        <v>-55.952184623932915</v>
+        <v>-55.952184578517404</v>
       </c>
     </row>
     <row r="78" spans="2:19" s="8" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -11358,31 +11358,31 @@
       </c>
       <c r="M79" s="54">
         <f t="shared" ca="1" si="22"/>
-        <v>-42.100531947610449</v>
+        <v>-42.100531947609831</v>
       </c>
       <c r="N79" s="54">
         <f t="shared" ca="1" si="22"/>
-        <v>-50.527262248956248</v>
+        <v>-50.527262248970089</v>
       </c>
       <c r="O79" s="54">
         <f t="shared" ca="1" si="22"/>
-        <v>-50.507725594779011</v>
+        <v>-50.507725594608317</v>
       </c>
       <c r="P79" s="54">
         <f t="shared" ca="1" si="22"/>
-        <v>-53.62206153680367</v>
+        <v>-53.622061538289728</v>
       </c>
       <c r="Q79" s="54">
         <f t="shared" ca="1" si="22"/>
-        <v>-82.758113058791054</v>
+        <v>-82.758113048377069</v>
       </c>
       <c r="R79" s="54">
         <f t="shared" ca="1" si="22"/>
-        <v>-88.308520245056968</v>
+        <v>-88.308520305059346</v>
       </c>
       <c r="S79" s="54">
         <f t="shared" ca="1" si="22"/>
-        <v>-94.081003438828546</v>
+        <v>-94.081003146935956</v>
       </c>
     </row>
     <row r="80" spans="2:19" s="8" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -11766,7 +11766,7 @@
       <pane xSplit="4" ySplit="4" topLeftCell="E5" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A61" sqref="A61"/>
-      <selection pane="bottomRight" activeCell="J6" sqref="J6"/>
+      <selection pane="bottomRight" activeCell="K9" sqref="K9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="15.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -15808,31 +15808,31 @@
       </c>
       <c r="M12" s="24">
         <f ca="1">'P&amp;L'!M27</f>
-        <v>38.482799907115151</v>
+        <v>38.482799907115208</v>
       </c>
       <c r="N12" s="24">
         <f ca="1">'P&amp;L'!N27</f>
-        <v>39.802833107755703</v>
+        <v>39.802833107754196</v>
       </c>
       <c r="O12" s="24">
         <f ca="1">'P&amp;L'!O27</f>
-        <v>55.340476300009698</v>
+        <v>55.340476300029451</v>
       </c>
       <c r="P12" s="64">
         <f ca="1">+'P&amp;L'!P27</f>
-        <v>82.126717322613899</v>
+        <v>82.126717322427055</v>
       </c>
       <c r="Q12" s="64">
         <f ca="1">+'P&amp;L'!Q27</f>
-        <v>88.847158753941812</v>
+        <v>88.847158755302303</v>
       </c>
       <c r="R12" s="64">
         <f ca="1">+'P&amp;L'!R27</f>
-        <v>95.532524970880957</v>
+        <v>95.532524962788955</v>
       </c>
       <c r="S12" s="64">
         <f ca="1">+'P&amp;L'!S27</f>
-        <v>103.42444214181467</v>
+        <v>103.42444218723017</v>
       </c>
     </row>
     <row r="14" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -18329,27 +18329,27 @@
       </c>
       <c r="N74">
         <f t="shared" ca="1" si="33"/>
-        <v>87.257242961995274</v>
+        <v>87.25724296199472</v>
       </c>
       <c r="O74">
         <f t="shared" ca="1" si="33"/>
-        <v>85.241903147267195</v>
+        <v>85.241903147281747</v>
       </c>
       <c r="P74">
         <f t="shared" ca="1" si="33"/>
-        <v>93.350029459650017</v>
+        <v>93.350029459442851</v>
       </c>
       <c r="Q74">
         <f t="shared" ca="1" si="33"/>
-        <v>119.54087853967529</v>
+        <v>119.54087854173562</v>
       </c>
       <c r="R74">
         <f t="shared" ca="1" si="33"/>
-        <v>149.53966745085461</v>
+        <v>149.53966743436553</v>
       </c>
       <c r="S74">
         <f t="shared" ca="1" si="33"/>
-        <v>183.29258541551306</v>
+        <v>183.29258552344811</v>
       </c>
     </row>
     <row r="75" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -18386,31 +18386,31 @@
       </c>
       <c r="M75" s="71">
         <f ca="1">+'P&amp;L'!M36</f>
-        <v>-2.0707570380053753</v>
+        <v>-2.0707570380052474</v>
       </c>
       <c r="N75" s="71">
         <f ca="1">+'P&amp;L'!N36</f>
-        <v>-2.0153398147101349</v>
+        <v>-2.0153398147133217</v>
       </c>
       <c r="O75" s="71">
         <f ca="1">+'P&amp;L'!O36</f>
-        <v>8.1081263121249911</v>
+        <v>8.1081263121661173</v>
       </c>
       <c r="P75" s="71">
         <f ca="1">+'P&amp;L'!P36</f>
-        <v>26.190849082612225</v>
+        <v>26.190849082236859</v>
       </c>
       <c r="Q75" s="71">
         <f ca="1">+'P&amp;L'!Q36</f>
-        <v>29.998788890465541</v>
+        <v>29.998788893125713</v>
       </c>
       <c r="R75" s="71">
         <f ca="1">+'P&amp;L'!R36</f>
-        <v>33.752918101560795</v>
+        <v>33.752918085417264</v>
       </c>
       <c r="S75" s="71">
         <f ca="1">+'P&amp;L'!S36</f>
-        <v>38.333923993747156</v>
+        <v>38.333924077567296</v>
       </c>
     </row>
     <row r="76" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -18564,31 +18564,31 @@
       </c>
       <c r="M78" s="62">
         <f t="shared" ca="1" si="35"/>
-        <v>87.257242961994592</v>
+        <v>87.257242961994734</v>
       </c>
       <c r="N78" s="62">
         <f t="shared" ca="1" si="35"/>
-        <v>85.241903147285143</v>
+        <v>85.241903147281391</v>
       </c>
       <c r="O78" s="62">
         <f t="shared" ca="1" si="35"/>
-        <v>93.350029459392189</v>
+        <v>93.350029459447867</v>
       </c>
       <c r="P78" s="62">
         <f t="shared" ca="1" si="35"/>
-        <v>119.54087854226225</v>
+        <v>119.54087854167972</v>
       </c>
       <c r="Q78" s="62">
         <f t="shared" ca="1" si="35"/>
-        <v>149.53966743014084</v>
+        <v>149.53966743486134</v>
       </c>
       <c r="R78" s="62">
         <f t="shared" ca="1" si="35"/>
-        <v>183.2925855524154</v>
+        <v>183.29258551978279</v>
       </c>
       <c r="S78" s="62">
         <f t="shared" ca="1" si="35"/>
-        <v>221.62650940926022</v>
+        <v>221.62650960101541</v>
       </c>
     </row>
     <row r="80" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -19836,31 +19836,31 @@
       </c>
       <c r="M107">
         <f t="shared" ca="1" si="50"/>
-        <v>-11.160011973063392</v>
+        <v>-11.16001197306341</v>
       </c>
       <c r="N107">
         <f t="shared" ca="1" si="50"/>
-        <v>-11.542821601249154</v>
+        <v>-11.542821601248717</v>
       </c>
       <c r="O107">
         <f t="shared" ca="1" si="50"/>
-        <v>-16.04873812700281</v>
+        <v>-16.048738127008541</v>
       </c>
       <c r="P107">
         <f t="shared" ca="1" si="50"/>
-        <v>-23.816748023558031</v>
+        <v>-23.816748023503845</v>
       </c>
       <c r="Q107">
         <f t="shared" ca="1" si="50"/>
-        <v>-25.765676038643125</v>
+        <v>-25.765676039037665</v>
       </c>
       <c r="R107">
         <f t="shared" ca="1" si="50"/>
-        <v>-27.704432241555477</v>
+        <v>-27.704432239208796</v>
       </c>
       <c r="S107">
         <f t="shared" ca="1" si="50"/>
-        <v>-29.99308822112625</v>
+        <v>-29.993088234296746</v>
       </c>
     </row>
     <row r="108" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -20363,31 +20363,31 @@
       </c>
       <c r="M13">
         <f t="shared" ref="M13:S13" ca="1" si="4">+M57</f>
-        <v>719.6797545840858</v>
+        <v>719.67975458408637</v>
       </c>
       <c r="N13">
         <f t="shared" ca="1" si="4"/>
-        <v>757.44874298172181</v>
+        <v>757.44874298170726</v>
       </c>
       <c r="O13">
         <f t="shared" ca="1" si="4"/>
-        <v>798.17734150147101</v>
+        <v>798.17734150167826</v>
       </c>
       <c r="P13">
         <f t="shared" ca="1" si="4"/>
-        <v>838.82718429161457</v>
+        <v>838.82718428955434</v>
       </c>
       <c r="Q13">
         <f t="shared" ca="1" si="4"/>
-        <v>852.63799745012523</v>
+        <v>852.63799746661437</v>
       </c>
       <c r="R13">
         <f t="shared" ca="1" si="4"/>
-        <v>862.34445301740561</v>
+        <v>862.34445290947031</v>
       </c>
       <c r="S13">
         <f t="shared" ca="1" si="4"/>
-        <v>867.49781722337082</v>
+        <v>867.49781781487332</v>
       </c>
     </row>
     <row r="14" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -20618,31 +20618,31 @@
       </c>
       <c r="M22">
         <f t="shared" ref="M22:S22" ca="1" si="6">+M41+M47+M53+M58+M65+M71</f>
-        <v>-46.609040079970399</v>
+        <v>-46.609040079970413</v>
       </c>
       <c r="N22">
         <f t="shared" ca="1" si="6"/>
-        <v>-48.876198931842609</v>
+        <v>-48.876198931842218</v>
       </c>
       <c r="O22">
         <f t="shared" ca="1" si="6"/>
-        <v>-51.074131365529389</v>
+        <v>-51.074131365534789</v>
       </c>
       <c r="P22">
         <f t="shared" ca="1" si="6"/>
-        <v>-53.352727722206389</v>
+        <v>-53.352727722154505</v>
       </c>
       <c r="Q22">
         <f t="shared" ca="1" si="6"/>
-        <v>-54.877626088768707</v>
+        <v>-54.877626089172722</v>
       </c>
       <c r="R22">
         <f t="shared" ca="1" si="6"/>
-        <v>-55.536109613090858</v>
+        <v>-55.536109610530367</v>
       </c>
       <c r="S22">
         <f t="shared" ca="1" si="6"/>
-        <v>-55.952184566741735</v>
+        <v>-55.95218458028161</v>
       </c>
     </row>
     <row r="24" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -20671,31 +20671,31 @@
       </c>
       <c r="M25" s="71">
         <f ca="1">+'BS &amp; CFS'!M65</f>
-        <v>70.477531947609776</v>
+        <v>70.477531947609847</v>
       </c>
       <c r="N25" s="71">
         <f ca="1">+'BS &amp; CFS'!N65</f>
-        <v>80.664262248971482</v>
+        <v>80.664262248969806</v>
       </c>
       <c r="O25" s="71">
         <f ca="1">+'BS &amp; CFS'!O65</f>
-        <v>83.669725594590716</v>
+        <v>83.669725594612089</v>
       </c>
       <c r="P25" s="71">
         <f ca="1">+'BS &amp; CFS'!P65</f>
-        <v>96.954818793861406</v>
+        <v>96.954818793672928</v>
       </c>
       <c r="Q25" s="71">
         <f ca="1">+'BS &amp; CFS'!Q65</f>
-        <v>128.30635661469557</v>
+        <v>128.30635661599524</v>
       </c>
       <c r="R25" s="71">
         <f ca="1">+'BS &amp; CFS'!R65</f>
-        <v>136.15414780832407</v>
+        <v>136.15414780027254</v>
       </c>
       <c r="S25" s="71">
         <f ca="1">+'BS &amp; CFS'!S65</f>
-        <v>144.42732943506977</v>
+        <v>144.4273294734744</v>
       </c>
     </row>
     <row r="26" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -20716,31 +20716,31 @@
       </c>
       <c r="M26" s="71">
         <f ca="1">+'P&amp;L'!M22</f>
-        <v>-46.609040079970477</v>
+        <v>-46.609040079970413</v>
       </c>
       <c r="N26" s="71">
         <f ca="1">+'P&amp;L'!N22</f>
-        <v>-48.87619893184074</v>
+        <v>-48.876198931842247</v>
       </c>
       <c r="O26" s="71">
         <f ca="1">+'P&amp;L'!O22</f>
-        <v>-51.074131365554045</v>
+        <v>-51.074131365534306</v>
       </c>
       <c r="P26" s="71">
         <f ca="1">+'P&amp;L'!P22</f>
-        <v>-53.352727721972769</v>
+        <v>-53.352727722159649</v>
       </c>
       <c r="Q26" s="71">
         <f ca="1">+'P&amp;L'!Q22</f>
-        <v>-54.877626090490274</v>
+        <v>-54.877626089129777</v>
       </c>
       <c r="R26" s="71">
         <f ca="1">+'P&amp;L'!R22</f>
-        <v>-55.536109602731841</v>
+        <v>-55.536109610823857</v>
       </c>
       <c r="S26" s="71">
         <f ca="1">+'P&amp;L'!S22</f>
-        <v>-55.952184623932915</v>
+        <v>-55.952184578517404</v>
       </c>
     </row>
     <row r="27" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -20903,31 +20903,31 @@
       </c>
       <c r="M30" s="62">
         <f t="shared" ca="1" si="8"/>
-        <v>-43.200970597800705</v>
+        <v>-43.200970597800563</v>
       </c>
       <c r="N30" s="62">
         <f t="shared" ca="1" si="8"/>
-        <v>-37.76898839761806</v>
+        <v>-37.768988397621243</v>
       </c>
       <c r="O30" s="62">
         <f t="shared" ca="1" si="8"/>
-        <v>-40.728598520007104</v>
+        <v>-40.728598519965992</v>
       </c>
       <c r="P30" s="62">
         <f t="shared" ca="1" si="8"/>
-        <v>-40.649842787556587</v>
+        <v>-40.649842787931945</v>
       </c>
       <c r="Q30" s="62">
         <f t="shared" ca="1" si="8"/>
-        <v>-13.810813179224345</v>
+        <v>-13.810813176564173</v>
       </c>
       <c r="R30" s="62">
         <f t="shared" ca="1" si="8"/>
-        <v>-9.7064554303779413</v>
+        <v>-9.7064554465214865</v>
       </c>
       <c r="S30" s="62">
         <f t="shared" ca="1" si="8"/>
-        <v>-5.1533649662639132</v>
+        <v>-5.153364882443773</v>
       </c>
     </row>
     <row r="32" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -21037,31 +21037,31 @@
       </c>
       <c r="M34">
         <f t="shared" ca="1" si="11"/>
-        <v>-43.200970597800712</v>
+        <v>-43.20097059780057</v>
       </c>
       <c r="N34">
         <f t="shared" ca="1" si="11"/>
-        <v>-37.768988397618067</v>
+        <v>-37.76898839762125</v>
       </c>
       <c r="O34">
         <f t="shared" ca="1" si="11"/>
-        <v>-40.728598520007111</v>
+        <v>-40.728598519965999</v>
       </c>
       <c r="P34">
         <f t="shared" ca="1" si="11"/>
-        <v>-40.649842787556594</v>
+        <v>-40.649842787931952</v>
       </c>
       <c r="Q34">
         <f t="shared" ca="1" si="11"/>
-        <v>-13.810813179224352</v>
+        <v>-13.81081317656418</v>
       </c>
       <c r="R34">
         <f t="shared" ca="1" si="11"/>
-        <v>-9.7064554303779484</v>
+        <v>-9.7064554465214936</v>
       </c>
       <c r="S34">
         <f t="shared" ca="1" si="11"/>
-        <v>-5.1533649662639203</v>
+        <v>-5.1533648824437801</v>
       </c>
     </row>
     <row r="36" spans="2:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -21793,27 +21793,27 @@
       </c>
       <c r="N55">
         <f t="shared" ca="1" si="25"/>
-        <v>719.6797545840858</v>
+        <v>719.67975458408637</v>
       </c>
       <c r="O55">
         <f t="shared" ca="1" si="25"/>
-        <v>757.44874298172181</v>
+        <v>757.44874298170726</v>
       </c>
       <c r="P55">
         <f t="shared" ca="1" si="25"/>
-        <v>798.17734150147101</v>
+        <v>798.17734150167826</v>
       </c>
       <c r="Q55">
         <f t="shared" ca="1" si="25"/>
-        <v>838.82718429161457</v>
+        <v>838.82718428955434</v>
       </c>
       <c r="R55">
         <f t="shared" ca="1" si="25"/>
-        <v>852.63799745012523</v>
+        <v>852.63799746661437</v>
       </c>
       <c r="S55">
         <f t="shared" ca="1" si="25"/>
-        <v>862.34445301740561</v>
+        <v>862.34445290947031</v>
       </c>
     </row>
     <row r="56" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -21834,31 +21834,31 @@
       </c>
       <c r="M56">
         <f t="shared" ca="1" si="26"/>
-        <v>43.200970597800712</v>
+        <v>43.20097059780057</v>
       </c>
       <c r="N56">
         <f t="shared" ca="1" si="26"/>
-        <v>37.768988397618067</v>
+        <v>37.76898839762125</v>
       </c>
       <c r="O56">
         <f t="shared" ca="1" si="26"/>
-        <v>40.728598520007111</v>
+        <v>40.728598519965999</v>
       </c>
       <c r="P56">
         <f t="shared" ca="1" si="26"/>
-        <v>40.649842787556594</v>
+        <v>40.649842787931952</v>
       </c>
       <c r="Q56">
         <f t="shared" ca="1" si="26"/>
-        <v>13.810813179224352</v>
+        <v>13.81081317656418</v>
       </c>
       <c r="R56">
         <f t="shared" ca="1" si="26"/>
-        <v>9.7064554303779484</v>
+        <v>9.7064554465214936</v>
       </c>
       <c r="S56">
         <f t="shared" ca="1" si="26"/>
-        <v>5.1533649662639203</v>
+        <v>5.1533648824437801</v>
       </c>
     </row>
     <row r="57" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -21889,31 +21889,31 @@
       </c>
       <c r="M57" s="62">
         <f t="shared" ca="1" si="27"/>
-        <v>719.67975458408648</v>
+        <v>719.67975458408637</v>
       </c>
       <c r="N57" s="62">
         <f t="shared" ca="1" si="27"/>
-        <v>757.44874298170384</v>
+        <v>757.4487429817076</v>
       </c>
       <c r="O57" s="62">
         <f t="shared" ca="1" si="27"/>
-        <v>798.17734150172896</v>
+        <v>798.17734150167325</v>
       </c>
       <c r="P57" s="62">
         <f t="shared" ca="1" si="27"/>
-        <v>838.82718428902763</v>
+        <v>838.82718428961016</v>
       </c>
       <c r="Q57" s="62">
         <f t="shared" ca="1" si="27"/>
-        <v>852.63799747083897</v>
+        <v>852.63799746611846</v>
       </c>
       <c r="R57" s="62">
         <f t="shared" ca="1" si="27"/>
-        <v>862.34445288050313</v>
+        <v>862.34445291313591</v>
       </c>
       <c r="S57" s="62">
         <f t="shared" ca="1" si="27"/>
-        <v>867.49781798366951</v>
+        <v>867.49781779191403</v>
       </c>
     </row>
     <row r="58" spans="1:19" s="2" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -21935,31 +21935,31 @@
       </c>
       <c r="M58" s="2">
         <f t="shared" ca="1" si="28"/>
-        <v>-39.092439079970426</v>
+        <v>-39.092439079970418</v>
       </c>
       <c r="N58" s="2">
         <f t="shared" ca="1" si="28"/>
-        <v>-41.359597931842131</v>
+        <v>-41.359597931842238</v>
       </c>
       <c r="O58" s="2">
         <f t="shared" ca="1" si="28"/>
-        <v>-43.557530365536117</v>
+        <v>-43.557530365534667</v>
       </c>
       <c r="P58" s="2">
         <f t="shared" ca="1" si="28"/>
-        <v>-45.836126722141188</v>
+        <v>-45.836126722155939</v>
       </c>
       <c r="Q58" s="2">
         <f t="shared" ca="1" si="28"/>
-        <v>-47.361025089276261</v>
+        <v>-47.361025089160407</v>
       </c>
       <c r="R58" s="2">
         <f t="shared" ca="1" si="28"/>
-        <v>-48.01950860983758</v>
+        <v>-48.01950861061912</v>
       </c>
       <c r="S58" s="2">
         <f t="shared" ca="1" si="28"/>
-        <v>-48.435583584196834</v>
+        <v>-48.435583579741397</v>
       </c>
     </row>
     <row r="59" spans="1:19" s="2" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -22461,7 +22461,7 @@
       <pane xSplit="4" ySplit="4" topLeftCell="E5" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A10" sqref="A10"/>
-      <selection pane="bottomRight" activeCell="E88" sqref="E88"/>
+      <selection pane="bottomRight" activeCell="F24" sqref="F24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="15.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -25230,7 +25230,7 @@
       </c>
       <c r="J34" s="71">
         <f ca="1">+'P&amp;L'!N62</f>
-        <v>112.02951758481946</v>
+        <v>112.02951758481916</v>
       </c>
     </row>
   </sheetData>

</xml_diff>